<commit_message>
task #47 Tests changed and reduced according to correct specifications: quotes should be added accordingly to existing cell style, no matter if underlying text "may be confused" with a number
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/leading_quotes.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/leading_quotes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Text</t>
   </si>
@@ -35,13 +35,7 @@
     <t>First two characters</t>
   </si>
   <si>
-    <t>123.456</t>
-  </si>
-  <si>
-    <t>123,456</t>
-  </si>
-  <si>
-    <t>pippo</t>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -363,7 +357,7 @@
   <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,16 +389,14 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C21" si="0">LEFT(B4,2)</f>
-        <v>12</v>
+        <v>ab</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v/>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -448,9 +440,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13" t="str">

</xml_diff>

<commit_message>
#47: Tests fixed and refactored
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/leading_quotes.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/leading_quotes.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\vaadin-spreadsheet\tagetik\tagetik-2017-spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27765" windowHeight="11250"/>
+    <workbookView xWindow="26000" yWindow="5080" windowWidth="19620" windowHeight="12880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Text</t>
   </si>
@@ -36,6 +39,18 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>Quote prepended string</t>
+  </si>
+  <si>
+    <t>Quote prepended string that looks like a number</t>
+  </si>
+  <si>
+    <t>String without quote</t>
+  </si>
+  <si>
+    <t>def</t>
   </si>
 </sst>
 </file>
@@ -76,7 +91,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -92,7 +107,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -137,9 +152,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -172,9 +187,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -354,19 +369,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F21"/>
+  <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -374,7 +390,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -383,115 +402,105 @@
         <v>01</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C21" si="0">LEFT(B4,2)</f>
+        <f t="shared" ref="C4:C18" si="0">LEFT(B4,2)</f>
         <v>ab</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>de</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C18" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>

</xml_diff>

<commit_message>
task #47 Create a specific test case to check the sheet-switch behaviour
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/leading_quotes.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/leading_quotes.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\vaadin-spreadsheet\tagetik\tagetik-2017-spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26000" yWindow="5080" windowWidth="19620" windowHeight="12880"/>
+    <workbookView xWindow="25995" yWindow="5085" windowWidth="19620" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Second sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -91,7 +92,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -375,14 +376,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -390,7 +391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -402,7 +403,7 @@
         <v>01</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -414,7 +415,7 @@
         <v>ab</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -426,80 +427,80 @@
         <v>de</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -508,4 +509,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>